<commit_message>
add final front index version
</commit_message>
<xml_diff>
--- a/URL IMAGES.xlsx
+++ b/URL IMAGES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Pierre\OneDrive\Documents\IUT\S3A\production\Projet\Application_Gestion_Easport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_53FD8BF9E8CCE15BB83B7D2FC8844F023199A49C" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_53FD8BF9E8CCE15BB83B7D2FC8844F023199A49C" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0AE5106C-8D10-4D8F-8077-FD0956B31377}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
   <si>
     <t>PERSONNAGE</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>ICONES</t>
+  </si>
+  <si>
+    <t>bonjout</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1285,7 @@
   <dimension ref="A1:H244"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1935,7 +1938,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1946,7 +1949,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1957,7 +1960,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1968,7 +1971,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1979,7 +1982,10 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="E37" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1990,7 +1996,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2001,7 +2007,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2012,7 +2018,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2023,7 +2029,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2034,7 +2040,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2045,7 +2051,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2056,7 +2062,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2067,7 +2073,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E45" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2078,7 +2084,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E46" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2089,7 +2095,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E47" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2100,7 +2106,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="5:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E48" s="2">
         <f t="shared" si="0"/>
         <v>47</v>

</xml_diff>